<commit_message>
Se modifico el achivo de configuración Config.xlsx
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,28 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmirabete\OneDrive\Documentos\UiPath\UNPA\RecoleccionCBA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54CF888-B2EC-468F-8C7E-8F2D31AAFE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -160,13 +173,148 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>URL_SitioSupermercado</t>
+  </si>
+  <si>
+    <t>URL base del portal comercial</t>
+  </si>
+  <si>
+    <t>Sucursal_BusquedaHabilitada</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>Indica si se debe seleccionar sucursal</t>
+  </si>
+  <si>
+    <t>Ruta_Input_Productos</t>
+  </si>
+  <si>
+    <t>Archivo con el listado de productos CBA</t>
+  </si>
+  <si>
+    <t>Ruta_Output_Resultados</t>
+  </si>
+  <si>
+    <t>Data\Output\Resultados_CBA.csv</t>
+  </si>
+  <si>
+    <t>Archivo CSV final generado por el robot</t>
+  </si>
+  <si>
+    <t>Ruta_Output_RegistroTiempos</t>
+  </si>
+  <si>
+    <t>Registro de inicio/fin del proceso</t>
+  </si>
+  <si>
+    <t>Ruta_Logs_Sesiones</t>
+  </si>
+  <si>
+    <t>Data\Logs\LogSesiones\</t>
+  </si>
+  <si>
+    <t>Carpeta para logs funcionales</t>
+  </si>
+  <si>
+    <t>Ruta_Logs_Errores</t>
+  </si>
+  <si>
+    <t>Data\Logs\LogErrores\</t>
+  </si>
+  <si>
+    <t>Carpeta para logs técnicos</t>
+  </si>
+  <si>
+    <t>Ruta_Screenshots</t>
+  </si>
+  <si>
+    <t>Screenshots\</t>
+  </si>
+  <si>
+    <t>Capturas para errores y excepciones</t>
+  </si>
+  <si>
+    <t>MaxRetriesBusiness</t>
+  </si>
+  <si>
+    <t>Negocio: no se reintenta</t>
+  </si>
+  <si>
+    <t>MaxRetriesSystem</t>
+  </si>
+  <si>
+    <t>Reintentos para errores de aplicación</t>
+  </si>
+  <si>
+    <t>TimeoutPagCarga</t>
+  </si>
+  <si>
+    <t>Timeout carga del sitio (ms)</t>
+  </si>
+  <si>
+    <t>TimeoutBusqueda</t>
+  </si>
+  <si>
+    <t>Timeout búsqueda por producto (ms)</t>
+  </si>
+  <si>
+    <t>TiempoEsperaResultados</t>
+  </si>
+  <si>
+    <t>Tiempo de espera para lista de productos</t>
+  </si>
+  <si>
+    <t>Correo_Notificaciones</t>
+  </si>
+  <si>
+    <t>martinmirabete@gmail.com</t>
+  </si>
+  <si>
+    <t>Dueño del proceso para alertas</t>
+  </si>
+  <si>
+    <t>https://www.laanonima.com.ar/</t>
+  </si>
+  <si>
+    <t>Sucursal_CodigoPostal</t>
+  </si>
+  <si>
+    <t>Código postal de la sucursal a seleccionar</t>
+  </si>
+  <si>
+    <t>Data\Input\Productos_CBA.csv</t>
+  </si>
+  <si>
+    <t>Data\Output\RegistroTiempos.csv</t>
+  </si>
+  <si>
+    <t>RIO GRANDE 4</t>
+  </si>
+  <si>
+    <t>AV.SAN MARTIN 1605</t>
+  </si>
+  <si>
+    <t>Sucursal_Denominacion</t>
+  </si>
+  <si>
+    <t>Sucursal_Domicilio</t>
+  </si>
+  <si>
+    <t>Denominación de la sucursal a seleccionar</t>
+  </si>
+  <si>
+    <t>Domicilio de la sucursal a seleccionar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +338,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,21 +368,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -239,9 +413,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +453,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +559,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -535,18 +709,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z984"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,7 +768,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +778,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -615,33 +789,205 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.5">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="8">
+        <v>9420</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="5">
+        <v>2</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="5">
+        <v>10000</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="5">
+        <v>5000</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="5">
+        <v>4000</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1594,24 +1940,13 @@
     <row r="982" ht="14.25" customHeight="1"/>
     <row r="983" ht="14.25" customHeight="1"/>
     <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" display="https://www.supermercado.com.ar" xr:uid="{9ECE8BE7-06DF-416E-98C5-50165BAB5C18}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1623,12 +1958,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +2000,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +2011,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +2125,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2782,14 +3117,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Se actualizaron las actividades del woekflow de negocio para registrar los logs.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmirabete\OneDrive\Documentos\UiPath\UNPA\RecoleccionCBA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54CF888-B2EC-468F-8C7E-8F2D31AAFE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8A99BC-B2A1-4713-8C88-5A31F9D38B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="147">
   <si>
     <t>Name</t>
   </si>
@@ -308,6 +308,177 @@
   </si>
   <si>
     <t>Domicilio de la sucursal a seleccionar</t>
+  </si>
+  <si>
+    <t>TituloProceso</t>
+  </si>
+  <si>
+    <t>Scraping de Precios CBA</t>
+  </si>
+  <si>
+    <t>Nombre del proceso</t>
+  </si>
+  <si>
+    <t>VersionProceso</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Versión para control</t>
+  </si>
+  <si>
+    <t>TiempoMinimoEntreTransacciones</t>
+  </si>
+  <si>
+    <t>Delay para evitar bloqueo del sitio</t>
+  </si>
+  <si>
+    <t>PrefijoCSV</t>
+  </si>
+  <si>
+    <t>CBA_</t>
+  </si>
+  <si>
+    <t>Prefijo para archivos de salida</t>
+  </si>
+  <si>
+    <t>UnidadMonetaria</t>
+  </si>
+  <si>
+    <t>ARS</t>
+  </si>
+  <si>
+    <t>Moneda para el precio</t>
+  </si>
+  <si>
+    <t>FormatoFechaSalida</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>Para logs y CSV</t>
+  </si>
+  <si>
+    <t>Selector_Buscador</t>
+  </si>
+  <si>
+    <t>"&lt;input name='search' /&gt;"</t>
+  </si>
+  <si>
+    <t>Selector del campo de búsqueda</t>
+  </si>
+  <si>
+    <t>Selector_ListaResultados</t>
+  </si>
+  <si>
+    <t>"//div[@class='product-list']"</t>
+  </si>
+  <si>
+    <t>Selector contenedor resultados</t>
+  </si>
+  <si>
+    <t>Selector_PrecioProducto</t>
+  </si>
+  <si>
+    <t>"//span[@class='price']"</t>
+  </si>
+  <si>
+    <t>Selector precio</t>
+  </si>
+  <si>
+    <t>Selector_ProductoLink</t>
+  </si>
+  <si>
+    <t>"//a[@class='product-link']"</t>
+  </si>
+  <si>
+    <t>Selector URL del producto</t>
+  </si>
+  <si>
+    <t>Correo_Origen</t>
+  </si>
+  <si>
+    <t>rpa@automatizaciones.local</t>
+  </si>
+  <si>
+    <t>Dirección usada para enviar correos</t>
+  </si>
+  <si>
+    <t>SMTP_Host</t>
+  </si>
+  <si>
+    <t>smtp.server.com</t>
+  </si>
+  <si>
+    <t>Servidor SMTP</t>
+  </si>
+  <si>
+    <t>SMTP_Port</t>
+  </si>
+  <si>
+    <t>Puerto SMTP</t>
+  </si>
+  <si>
+    <t>SMTP_UseSSL</t>
+  </si>
+  <si>
+    <t>Seguridad para correos</t>
+  </si>
+  <si>
+    <t>CantidadTotalProductosEsperados</t>
+  </si>
+  <si>
+    <t>Control de calidad del volumen</t>
+  </si>
+  <si>
+    <t>ValidarFormatoPrecio</t>
+  </si>
+  <si>
+    <t>Habilita chequeo de formato</t>
+  </si>
+  <si>
+    <t>RegistrarProductoAmbiguo</t>
+  </si>
+  <si>
+    <t>PRIMERO_LISTA</t>
+  </si>
+  <si>
+    <t>Acción según PDD</t>
+  </si>
+  <si>
+    <t>GenerarCSVFinal</t>
+  </si>
+  <si>
+    <t>Indica si debe generar el CSV</t>
+  </si>
+  <si>
+    <t>FechaEjecucion</t>
+  </si>
+  <si>
+    <t>Fecha para reportes</t>
+  </si>
+  <si>
+    <t>ActivarScreenshotErrores</t>
+  </si>
+  <si>
+    <t>Captura pantalla en errores</t>
+  </si>
+  <si>
+    <t>ActivarScreenshotNegocio</t>
+  </si>
+  <si>
+    <t>Captura pantalla en excepciones conocidas</t>
+  </si>
+  <si>
+    <t>VerboseLog</t>
+  </si>
+  <si>
+    <t>Detalla cada paso del robot</t>
+  </si>
+  <si>
+    <t>=TODAY()</t>
   </si>
 </sst>
 </file>
@@ -372,7 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,6 +565,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -709,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z984"/>
+  <dimension ref="A1:Z983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -969,41 +1141,201 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="A23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C27" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30">
+        <v>587</v>
+      </c>
+      <c r="C30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32">
+        <v>200</v>
+      </c>
+      <c r="C32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -1939,7 +2271,6 @@
     <row r="981" ht="14.25" customHeight="1"/>
     <row r="982" ht="14.25" customHeight="1"/>
     <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -1954,8 +2285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2137,12 +2468,72 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21">
+        <v>250</v>
+      </c>
+      <c r="C21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3117,7 +3508,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
Se implemento correctamente la verificación de URL y la apertura del navegador en el sitio del supermercado.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmirabete\OneDrive\Documentos\UiPath\UNPA\RecoleccionCBA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8A99BC-B2A1-4713-8C88-5A31F9D38B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B537EE49-0835-4ACB-A49B-184264E417EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -277,9 +277,6 @@
     <t>Dueño del proceso para alertas</t>
   </si>
   <si>
-    <t>https://www.laanonima.com.ar/</t>
-  </si>
-  <si>
     <t>Sucursal_CodigoPostal</t>
   </si>
   <si>
@@ -479,6 +476,9 @@
   </si>
   <si>
     <t>=TODAY()</t>
+  </si>
+  <si>
+    <t>https://www.laanonima.com.ar/buscar/</t>
   </si>
 </sst>
 </file>
@@ -883,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -969,7 +969,7 @@
         <v>45</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>79</v>
+        <v>146</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>46</v>
@@ -988,35 +988,35 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="8">
         <v>9420</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -1024,7 +1024,7 @@
         <v>50</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>51</v>
@@ -1046,7 +1046,7 @@
         <v>55</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>56</v>
@@ -1142,46 +1142,46 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" t="s">
         <v>107</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>108</v>
-      </c>
-      <c r="C23" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" t="s">
         <v>110</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>111</v>
-      </c>
-      <c r="C24" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" t="s">
         <v>113</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>114</v>
-      </c>
-      <c r="C25" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" t="s">
         <v>116</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>117</v>
-      </c>
-      <c r="C26" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
@@ -1197,134 +1197,134 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" t="s">
         <v>119</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>120</v>
-      </c>
-      <c r="C28" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" t="s">
         <v>122</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>123</v>
-      </c>
-      <c r="C29" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B30">
         <v>587</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
         <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B32">
         <v>200</v>
       </c>
       <c r="C32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B33" t="s">
         <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" t="s">
         <v>133</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>134</v>
-      </c>
-      <c r="C34" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
         <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" t="s">
         <v>138</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="C36" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
         <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B38" t="s">
         <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B39" t="s">
         <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2274,7 +2274,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" display="https://www.supermercado.com.ar" xr:uid="{9ECE8BE7-06DF-416E-98C5-50165BAB5C18}"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{9ECE8BE7-06DF-416E-98C5-50165BAB5C18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2470,68 +2470,68 @@
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" t="s">
         <v>90</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>91</v>
-      </c>
-      <c r="C19" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" t="s">
         <v>93</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>94</v>
-      </c>
-      <c r="C20" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21">
         <v>250</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" t="s">
         <v>98</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>99</v>
-      </c>
-      <c r="C22" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" t="s">
         <v>101</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>102</v>
-      </c>
-      <c r="C23" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" t="s">
         <v>104</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>105</v>
-      </c>
-      <c r="C24" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Se implemento la selección de sucursal
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmirabete\OneDrive\Documentos\UiPath\UNPA\RecoleccionCBA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B537EE49-0835-4ACB-A49B-184264E417EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950DFA5C-BCF0-4AA7-B3B5-CDDEF9ED4D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="150">
   <si>
     <t>Name</t>
   </si>
@@ -478,7 +478,16 @@
     <t>=TODAY()</t>
   </si>
   <si>
-    <t>https://www.laanonima.com.ar/buscar/</t>
+    <t>buscar/</t>
+  </si>
+  <si>
+    <t>https://www.laanonima.com.ar/</t>
+  </si>
+  <si>
+    <t>URL_SitioSupermercado_SeccionBusqueda</t>
+  </si>
+  <si>
+    <t>URL de la sección de búsqueda del portal comercial</t>
   </si>
 </sst>
 </file>
@@ -881,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z983"/>
+  <dimension ref="A1:Z984"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -969,7 +978,7 @@
         <v>45</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>46</v>
@@ -977,357 +986,367 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>48</v>
+        <v>148</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>49</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="8">
-        <v>9420</v>
+        <v>47</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="B10" s="8">
+        <v>9420</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="5">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B19" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B20" s="5">
-        <v>10000</v>
+        <v>2</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B21" s="5">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="5">
+        <v>5000</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B23" s="5">
         <v>4000</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B23" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B25" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>124</v>
-      </c>
-      <c r="B30">
-        <v>587</v>
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
+        <v>122</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" t="s">
-        <v>48</v>
+        <v>124</v>
+      </c>
+      <c r="B31">
+        <v>587</v>
       </c>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>128</v>
-      </c>
-      <c r="B32">
-        <v>200</v>
+        <v>126</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33" t="s">
-        <v>48</v>
+        <v>128</v>
+      </c>
+      <c r="B33">
+        <v>200</v>
       </c>
       <c r="C33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B34" t="s">
-        <v>133</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
       <c r="C35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>137</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>145</v>
+        <v>135</v>
+      </c>
+      <c r="B36" t="s">
+        <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>139</v>
-      </c>
-      <c r="B37" t="s">
-        <v>48</v>
+        <v>137</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B38" t="s">
         <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B39" t="s">
         <v>48</v>
       </c>
       <c r="C39" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A40" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2271,13 +2290,15 @@
     <row r="981" ht="14.25" customHeight="1"/>
     <row r="982" ht="14.25" customHeight="1"/>
     <row r="983" ht="14.25" customHeight="1"/>
+    <row r="984" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9ECE8BE7-06DF-416E-98C5-50165BAB5C18}"/>
+    <hyperlink ref="B8" r:id="rId2" display="https://www.laanonima.com.ar/buscar/" xr:uid="{06B68689-7BCD-4301-80A3-3BC470270DD1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>